<commit_message>
Actualización de boot -SG
</commit_message>
<xml_diff>
--- a/Frecuentista_depto/COL/Output/Comparando_dir_censo_sae/Estimacion_depto.xlsx
+++ b/Frecuentista_depto/COL/Output/Comparando_dir_censo_sae/Estimacion_depto.xlsx
@@ -12,27 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">depto</t>
   </si>
   <si>
+    <t xml:space="preserve">nd</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dir_Educacion</t>
   </si>
   <si>
-    <t xml:space="preserve">Dir_Educacion_se</t>
+    <t xml:space="preserve">Dir_Educacion_cv</t>
   </si>
   <si>
     <t xml:space="preserve">Dir_Empleo</t>
   </si>
   <si>
-    <t xml:space="preserve">Dir_Empleo_se</t>
+    <t xml:space="preserve">Dir_Empleo_cv</t>
   </si>
   <si>
     <t xml:space="preserve">Dir_IPM</t>
   </si>
   <si>
-    <t xml:space="preserve">Dir_IPM_se</t>
+    <t xml:space="preserve">Dir_IPM_cv</t>
   </si>
   <si>
     <t xml:space="preserve">sae_MC_Educacion</t>
@@ -575,1642 +578,1717 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" t="n">
+        <v>35264</v>
+      </c>
+      <c r="C2" t="n">
         <v>0.646031468946502</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.00312340971523757</v>
-      </c>
       <c r="D2" t="n">
+        <v>0.0122363159273592</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.492689294407173</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.00337419355242385</v>
-      </c>
       <c r="F2" t="n">
-        <v>0.34151893142224</v>
+        <v>0.0234368227720502</v>
       </c>
       <c r="G2" t="n">
-        <v>0.001634280872511</v>
+        <v>0.455453832969968</v>
       </c>
       <c r="H2" t="n">
+        <v>0.0432303687012702</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.649198730991558</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.488201967721922</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.473842788633127</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.00231176578588815</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.00236655069326775</v>
       </c>
-      <c r="M2" t="n">
-        <v>0.135675479443519</v>
-      </c>
       <c r="N2" t="n">
+        <v>0.00152529850382078</v>
+      </c>
+      <c r="O2" t="n">
         <v>0.364534091071495</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0.473526519500823</v>
       </c>
-      <c r="P2" t="n">
-        <v>28.6330155693402</v>
-      </c>
       <c r="Q2" t="n">
+        <v>0.321899697623498</v>
+      </c>
+      <c r="R2" t="n">
         <v>0.644560291632753</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>0.653837170350363</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.483670906781581</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.492733028662263</v>
       </c>
-      <c r="U2" t="n">
-        <v>0.20791884892383</v>
-      </c>
       <c r="V2" t="n">
-        <v>0.739766728342424</v>
+        <v>0.470853203565638</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.476832373700615</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="n">
+        <v>31445</v>
+      </c>
+      <c r="C3" t="n">
         <v>0.531246079338757</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.00342960650042224</v>
-      </c>
       <c r="D3" t="n">
+        <v>0.0102559205399277</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.616411361201528</v>
       </c>
-      <c r="E3" t="n">
-        <v>0.00323763079965608</v>
-      </c>
       <c r="F3" t="n">
-        <v>0.335585381756959</v>
+        <v>0.0102454935547865</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0014843437560653</v>
+        <v>0.453295906236899</v>
       </c>
       <c r="H3" t="n">
+        <v>0.016948506765515</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.542272216357288</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.60088414031413</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.460791351757007</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.00235600679767414</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.00273222834405392</v>
       </c>
-      <c r="M3" t="n">
-        <v>0.135198094040841</v>
-      </c>
       <c r="N3" t="n">
+        <v>0.00163651724101988</v>
+      </c>
+      <c r="O3" t="n">
         <v>0.503848115695039</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.392090028610584</v>
       </c>
-      <c r="P3" t="n">
-        <v>29.3404148158007</v>
-      </c>
       <c r="Q3" t="n">
+        <v>0.355153636191262</v>
+      </c>
+      <c r="R3" t="n">
         <v>0.536917048802942</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.547627383911633</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>0.596266366990689</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.605501913637572</v>
       </c>
-      <c r="U3" t="n">
-        <v>0.195803087436958</v>
-      </c>
       <c r="V3" t="n">
-        <v>0.725779616077056</v>
+        <v>0.457583777964608</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.463998925549406</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="n">
+        <v>24594</v>
+      </c>
+      <c r="C4" t="n">
         <v>0.573541855393646</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.00324302296993449</v>
-      </c>
       <c r="D4" t="n">
+        <v>0.00639841023975061</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.427985524029992</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.00324941988151148</v>
-      </c>
       <c r="F4" t="n">
-        <v>0.2539726100172</v>
+        <v>0.00870340887289321</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00106456658878392</v>
+        <v>0.284482254225353</v>
       </c>
       <c r="H4" t="n">
+        <v>0.0161562512835023</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.58431274528565</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.408652337854738</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.279988761045496</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0.00316367984963938</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>0.00279248261528358</v>
       </c>
-      <c r="M4" t="n">
-        <v>0.0581384868268255</v>
-      </c>
       <c r="N4" t="n">
+        <v>0.00203363406715498</v>
+      </c>
+      <c r="O4" t="n">
         <v>0.477908900295925</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>0.774173926484169</v>
       </c>
-      <c r="P4" t="n">
-        <v>20.7645787672807</v>
-      </c>
       <c r="Q4" t="n">
+        <v>0.726327035257149</v>
+      </c>
+      <c r="R4" t="n">
         <v>0.578839479359694</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>0.589786011211606</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>0.402451525349445</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>0.414853150360031</v>
       </c>
-      <c r="U4" t="n">
-        <v>0.166037326864918</v>
-      </c>
       <c r="V4" t="n">
-        <v>0.393940195226074</v>
+        <v>0.276002838273873</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.28397468381712</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="n">
+        <v>24837</v>
+      </c>
+      <c r="C5" t="n">
         <v>0.652883565191465</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.00451269146050949</v>
-      </c>
       <c r="D5" t="n">
+        <v>0.0133588636411288</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.671537453556966</v>
       </c>
-      <c r="E5" t="n">
-        <v>0.0042405102626164</v>
-      </c>
       <c r="F5" t="n">
-        <v>0.449986684436791</v>
+        <v>0.0155427096797639</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00246710245169869</v>
+        <v>0.631695350572367</v>
       </c>
       <c r="H5" t="n">
+        <v>0.0220955045120061</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.647318447403382</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>0.641599854107281</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.632623940737174</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0.00257243083110167</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>0.00281627144216852</v>
       </c>
-      <c r="M5" t="n">
-        <v>0.215338968844249</v>
-      </c>
       <c r="N5" t="n">
+        <v>0.00144522402218597</v>
+      </c>
+      <c r="O5" t="n">
         <v>0.435067385066123</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>0.400940058610353</v>
       </c>
-      <c r="P5" t="n">
-        <v>34.0390167013474</v>
-      </c>
       <c r="Q5" t="n">
+        <v>0.228449151086806</v>
+      </c>
+      <c r="R5" t="n">
         <v>0.641798555376732</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>0.652838339430032</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>0.636557889678322</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>0.646641818536241</v>
       </c>
-      <c r="U5" t="n">
-        <v>0.210559561802447</v>
-      </c>
       <c r="V5" t="n">
-        <v>1.0546883196719</v>
+        <v>0.629791301653689</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.635456579820658</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="n">
+        <v>19312</v>
+      </c>
+      <c r="C6" t="n">
         <v>0.667923343012017</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.00683728374472864</v>
-      </c>
       <c r="D6" t="n">
+        <v>0.0137434547594035</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.610926546733503</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.00684865157511168</v>
-      </c>
       <c r="F6" t="n">
-        <v>0.410857300068537</v>
+        <v>0.0247331419747194</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00278885867073024</v>
+        <v>0.615385585877384</v>
       </c>
       <c r="H6" t="n">
+        <v>0.0409827146443487</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.699363159911048</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>0.584669548600328</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.631192968656138</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0.00308566566691175</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>0.00318674057032065</v>
       </c>
-      <c r="M6" t="n">
-        <v>0.212810850633746</v>
-      </c>
       <c r="N6" t="n">
+        <v>0.00158374034307516</v>
+      </c>
+      <c r="O6" t="n">
         <v>0.455663202323378</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>0.527762335886774</v>
       </c>
-      <c r="P6" t="n">
-        <v>33.7156560990908</v>
-      </c>
       <c r="Q6" t="n">
+        <v>0.250912228386681</v>
+      </c>
+      <c r="R6" t="n">
         <v>0.69311714839322</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>0.705609171428877</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>0.578621643893181</v>
       </c>
-      <c r="T6" t="n">
+      <c r="U6" t="n">
         <v>0.590717453307475</v>
       </c>
-      <c r="U6" t="n">
-        <v>0.214083701413996</v>
-      </c>
       <c r="V6" t="n">
-        <v>1.04830223589828</v>
+        <v>0.62808883758371</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.634297099728565</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" t="n">
+        <v>24139</v>
+      </c>
+      <c r="C7" t="n">
         <v>0.643218101194196</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.00569822112838802</v>
-      </c>
       <c r="D7" t="n">
+        <v>0.0161790037431009</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.535410487497843</v>
       </c>
-      <c r="E7" t="n">
-        <v>0.00594284790996504</v>
-      </c>
       <c r="F7" t="n">
-        <v>0.371766285833273</v>
+        <v>0.0339916807302881</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00247397471906232</v>
+        <v>0.521485471371696</v>
       </c>
       <c r="H7" t="n">
+        <v>0.0533490420681228</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.623141254306129</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.489618402585804</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>0.490201736805172</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0.00261840705503407</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>0.00334827073445093</v>
       </c>
-      <c r="M7" t="n">
-        <v>0.124448274891151</v>
-      </c>
       <c r="N7" t="n">
+        <v>0.0017627812798319</v>
+      </c>
+      <c r="O7" t="n">
         <v>0.537321307378252</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>0.534785261584445</v>
       </c>
-      <c r="P7" t="n">
-        <v>25.3871550317685</v>
-      </c>
       <c r="Q7" t="n">
+        <v>0.359603230155936</v>
+      </c>
+      <c r="R7" t="n">
         <v>0.616578643666605</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>0.629703864945652</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>0.484486324757937</v>
       </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
         <v>0.49475048041367</v>
       </c>
-      <c r="U7" t="n">
-        <v>0.246283118018516</v>
-      </c>
       <c r="V7" t="n">
-        <v>0.734120355591827</v>
+        <v>0.486746685496701</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.493656788113642</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="n">
+        <v>19117</v>
+      </c>
+      <c r="C8" t="n">
         <v>0.72213008434979</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.00630048534681465</v>
-      </c>
       <c r="D8" t="n">
+        <v>0.0163753716614274</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.763437135211824</v>
       </c>
-      <c r="E8" t="n">
-        <v>0.00540974407988803</v>
-      </c>
       <c r="F8" t="n">
-        <v>0.512964415775196</v>
+        <v>0.0144538919809412</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00234375249632998</v>
+        <v>0.796493205161876</v>
       </c>
       <c r="H8" t="n">
+        <v>0.0163780251745944</v>
+      </c>
+      <c r="I8" t="n">
         <v>0.746260244142302</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>0.722996518942883</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>0.774046143519458</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>0.00314253548686994</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>0.00321848395386037</v>
       </c>
-      <c r="M8" t="n">
-        <v>0.191256596210678</v>
-      </c>
       <c r="N8" t="n">
+        <v>0.00171343199599288</v>
+      </c>
+      <c r="O8" t="n">
         <v>0.431281711591038</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>0.434654303932852</v>
       </c>
-      <c r="P8" t="n">
-        <v>24.708681492949</v>
-      </c>
       <c r="Q8" t="n">
+        <v>0.221360446058448</v>
+      </c>
+      <c r="R8" t="n">
         <v>0.739952015592735</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>0.752568472691868</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>0.716837149388617</v>
       </c>
-      <c r="T8" t="n">
+      <c r="U8" t="n">
         <v>0.729155888497148</v>
       </c>
-      <c r="U8" t="n">
-        <v>0.39918321494653</v>
-      </c>
       <c r="V8" t="n">
-        <v>1.14890907209239</v>
+        <v>0.770687816807312</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.777404470231604</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="n">
+        <v>25641</v>
+      </c>
+      <c r="C9" t="n">
         <v>0.667383179365901</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.00612034917889904</v>
-      </c>
       <c r="D9" t="n">
+        <v>0.020919322646248</v>
+      </c>
+      <c r="E9" t="n">
         <v>0.706238725903718</v>
       </c>
-      <c r="E9" t="n">
-        <v>0.0055911868945922</v>
-      </c>
       <c r="F9" t="n">
-        <v>0.491833693290234</v>
+        <v>0.0200125432188873</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00255719513074153</v>
+        <v>0.736748961415124</v>
       </c>
       <c r="H9" t="n">
+        <v>0.0237836869092163</v>
+      </c>
+      <c r="I9" t="n">
         <v>0.739854415825333</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>0.718035372338152</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0.792234563204733</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>0.0023030426190356</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>0.00264247241616706</v>
       </c>
-      <c r="M9" t="n">
-        <v>0.210623869643663</v>
-      </c>
       <c r="N9" t="n">
+        <v>0.00115603457025226</v>
+      </c>
+      <c r="O9" t="n">
         <v>0.357161133277727</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>0.320742223539233</v>
       </c>
-      <c r="P9" t="n">
-        <v>26.5860490599717</v>
-      </c>
       <c r="Q9" t="n">
+        <v>0.14592074417656</v>
+      </c>
+      <c r="R9" t="n">
         <v>0.734675169889646</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>0.745033661761021</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>0.713521408804842</v>
       </c>
-      <c r="T9" t="n">
+      <c r="U9" t="n">
         <v>0.722549335871462</v>
       </c>
-      <c r="U9" t="n">
-        <v>0.379411778703154</v>
-      </c>
       <c r="V9" t="n">
-        <v>1.20505734770631</v>
+        <v>0.789968735447038</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.794500390962427</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" t="n">
+        <v>21789</v>
+      </c>
+      <c r="C10" t="n">
         <v>0.669223003220315</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.00542303480665617</v>
-      </c>
       <c r="D10" t="n">
+        <v>0.0151098190021899</v>
+      </c>
+      <c r="E10" t="n">
         <v>0.706879692595728</v>
       </c>
-      <c r="E10" t="n">
-        <v>0.00519520727478836</v>
-      </c>
       <c r="F10" t="n">
-        <v>0.460910295258274</v>
+        <v>0.0124185107950698</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0030205892224955</v>
+        <v>0.662764350369233</v>
       </c>
       <c r="H10" t="n">
+        <v>0.0227072693332446</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.649918885562665</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>0.705526558186348</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.659700510490542</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0.00244571428180775</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>0.00289923695065701</v>
       </c>
-      <c r="M10" t="n">
-        <v>0.229838728344693</v>
-      </c>
       <c r="N10" t="n">
+        <v>0.00186660483346259</v>
+      </c>
+      <c r="O10" t="n">
         <v>0.446092122426478</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>0.346650916741503</v>
       </c>
-      <c r="P10" t="n">
-        <v>34.8398591011835</v>
-      </c>
       <c r="Q10" t="n">
+        <v>0.282947307722198</v>
+      </c>
+      <c r="R10" t="n">
         <v>0.644236381139377</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>0.655601389985953</v>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>0.700732958194005</v>
       </c>
-      <c r="T10" t="n">
+      <c r="U10" t="n">
         <v>0.710320158178692</v>
       </c>
-      <c r="U10" t="n">
-        <v>0.209216602934943</v>
-      </c>
       <c r="V10" t="n">
-        <v>1.11018441804614</v>
+        <v>0.656041965016955</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.663359055964128</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" t="n">
+        <v>22387</v>
+      </c>
+      <c r="C11" t="n">
         <v>0.633572227796042</v>
       </c>
-      <c r="C11" t="n">
-        <v>0.00717444503002695</v>
-      </c>
       <c r="D11" t="n">
+        <v>0.0148768169633349</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.733469683582859</v>
       </c>
-      <c r="E11" t="n">
-        <v>0.00624305620661582</v>
-      </c>
       <c r="F11" t="n">
-        <v>0.503954027206085</v>
+        <v>0.0119871335787648</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00343600815634537</v>
+        <v>0.714470429787794</v>
       </c>
       <c r="H11" t="n">
+        <v>0.0234502470624658</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.643772520705782</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>0.719430138097316</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0.729332548739581</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0.00232868099212124</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>0.0027343908310323</v>
       </c>
-      <c r="M11" t="n">
-        <v>0.187851850948922</v>
-      </c>
       <c r="N11" t="n">
+        <v>0.00141325446373689</v>
+      </c>
+      <c r="O11" t="n">
         <v>0.424744881629078</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>0.323684103404388</v>
       </c>
-      <c r="P11" t="n">
-        <v>25.7566800321148</v>
-      </c>
       <c r="Q11" t="n">
+        <v>0.193773672404892</v>
+      </c>
+      <c r="R11" t="n">
         <v>0.638413114676958</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>0.649131926734605</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>0.714865923352758</v>
       </c>
-      <c r="T11" t="n">
+      <c r="U11" t="n">
         <v>0.723994352841874</v>
       </c>
-      <c r="U11" t="n">
-        <v>0.361142920879695</v>
-      </c>
       <c r="V11" t="n">
-        <v>1.09752217659947</v>
+        <v>0.726562569990657</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.732102527488505</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" t="n">
+        <v>6613</v>
+      </c>
+      <c r="C12" t="n">
         <v>0.615507923256318</v>
       </c>
-      <c r="C12" t="n">
-        <v>0.00668116195044933</v>
-      </c>
       <c r="D12" t="n">
+        <v>0.0131978838012724</v>
+      </c>
+      <c r="E12" t="n">
         <v>0.56398402183457</v>
       </c>
-      <c r="E12" t="n">
-        <v>0.00678756737693442</v>
-      </c>
       <c r="F12" t="n">
-        <v>0.381873443557483</v>
+        <v>0.0296568739387281</v>
       </c>
       <c r="G12" t="n">
-        <v>0.00289659297104646</v>
+        <v>0.552134997456974</v>
       </c>
       <c r="H12" t="n">
+        <v>0.0374849182064167</v>
+      </c>
+      <c r="I12" t="n">
         <v>0.62065986148731</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>0.530861890919076</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>0.481205105399773</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>0.00631395726223987</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>0.00543972911234428</v>
       </c>
-      <c r="M12" t="n">
-        <v>0.158985275362944</v>
-      </c>
       <c r="N12" t="n">
+        <v>0.003854835838318</v>
+      </c>
+      <c r="O12" t="n">
         <v>0.876442871512402</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>1.18937851261249</v>
       </c>
-      <c r="P12" t="n">
-        <v>33.0389834976633</v>
-      </c>
       <c r="Q12" t="n">
+        <v>0.801079580216736</v>
+      </c>
+      <c r="R12" t="n">
         <v>0.609997992427115</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>0.631321730547505</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>0.518486534685086</v>
       </c>
-      <c r="T12" t="n">
+      <c r="U12" t="n">
         <v>0.543237247153066</v>
       </c>
-      <c r="U12" t="n">
-        <v>0.169593965688402</v>
-      </c>
       <c r="V12" t="n">
-        <v>0.792816245111143</v>
+        <v>0.473649627156669</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.488760583642876</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" t="n">
+        <v>16900</v>
+      </c>
+      <c r="C13" t="n">
         <v>0.716158353532741</v>
       </c>
-      <c r="C13" t="n">
-        <v>0.00724712123177308</v>
-      </c>
       <c r="D13" t="n">
+        <v>0.0199853842235368</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.753839305688845</v>
       </c>
-      <c r="E13" t="n">
-        <v>0.00677856502184301</v>
-      </c>
       <c r="F13" t="n">
-        <v>0.630498054155879</v>
+        <v>0.0191776743361688</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00303626152623907</v>
+        <v>0.927914308185246</v>
       </c>
       <c r="H13" t="n">
+        <v>0.014034897498135</v>
+      </c>
+      <c r="I13" t="n">
         <v>0.766862976337199</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>0.720300709917248</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>0.929001763996532</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0.00319887393836746</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>0.00309196118596838</v>
       </c>
-      <c r="M13" t="n">
-        <v>0.135650403714869</v>
-      </c>
       <c r="N13" t="n">
+        <v>0.000857581250868223</v>
+      </c>
+      <c r="O13" t="n">
         <v>0.403196044322891</v>
       </c>
-      <c r="O13" t="n">
+      <c r="P13" t="n">
         <v>0.444102566376057</v>
       </c>
-      <c r="P13" t="n">
-        <v>14.6017380129942</v>
-      </c>
       <c r="Q13" t="n">
+        <v>0.092312122980148</v>
+      </c>
+      <c r="R13" t="n">
         <v>0.760802732412701</v>
       </c>
-      <c r="R13" t="n">
+      <c r="S13" t="n">
         <v>0.772923220261697</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>0.714030916998048</v>
       </c>
-      <c r="T13" t="n">
+      <c r="U13" t="n">
         <v>0.726570502836449</v>
       </c>
-      <c r="U13" t="n">
-        <v>0.663126972715389</v>
-      </c>
       <c r="V13" t="n">
-        <v>1.19487655527767</v>
+        <v>0.92732090474483</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.930682623248233</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" t="n">
+        <v>21882</v>
+      </c>
+      <c r="C14" t="n">
         <v>0.674345694284293</v>
       </c>
-      <c r="C14" t="n">
-        <v>0.00638028242198464</v>
-      </c>
       <c r="D14" t="n">
+        <v>0.0112708711710327</v>
+      </c>
+      <c r="E14" t="n">
         <v>0.678515266920817</v>
       </c>
-      <c r="E14" t="n">
-        <v>0.00591065918660441</v>
-      </c>
       <c r="F14" t="n">
-        <v>0.423465467280836</v>
+        <v>0.0181938890757664</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0027304938367022</v>
+        <v>0.613260439316588</v>
       </c>
       <c r="H14" t="n">
+        <v>0.0302998226552923</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.682143343498224</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>0.665732600684077</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>0.633568644801997</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0.00252262354389423</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>0.00305906564565818</v>
       </c>
-      <c r="M14" t="n">
-        <v>0.199890021605445</v>
-      </c>
       <c r="N14" t="n">
+        <v>0.00173393111915598</v>
+      </c>
+      <c r="O14" t="n">
         <v>0.448449094287196</v>
       </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
         <v>0.378924442231324</v>
       </c>
-      <c r="P14" t="n">
-        <v>31.5498601841186</v>
-      </c>
       <c r="Q14" t="n">
+        <v>0.273676914629806</v>
+      </c>
+      <c r="R14" t="n">
         <v>0.676147574832734</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
         <v>0.688139112163714</v>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>0.660788258538044</v>
       </c>
-      <c r="T14" t="n">
+      <c r="U14" t="n">
         <v>0.670676942830109</v>
       </c>
-      <c r="U14" t="n">
-        <v>0.241784202455325</v>
-      </c>
       <c r="V14" t="n">
-        <v>1.02535308714867</v>
+        <v>0.630170139808451</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.636967149795542</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" t="n">
+        <v>22516</v>
+      </c>
+      <c r="C15" t="n">
         <v>0.720280981493297</v>
       </c>
-      <c r="C15" t="n">
-        <v>0.0070961158152643</v>
-      </c>
       <c r="D15" t="n">
+        <v>0.0190851050289625</v>
+      </c>
+      <c r="E15" t="n">
         <v>0.761909547287528</v>
       </c>
-      <c r="E15" t="n">
-        <v>0.00658107805984963</v>
-      </c>
       <c r="F15" t="n">
-        <v>0.592430158975899</v>
+        <v>0.0208995086789547</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00374060054228859</v>
+        <v>0.823982459272416</v>
       </c>
       <c r="H15" t="n">
+        <v>0.0185139071518655</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.780488510496068</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>0.790418598605476</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>0.829540995478474</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>0.0020721419568032</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>0.00281137806399219</v>
       </c>
-      <c r="M15" t="n">
-        <v>0.182031513646177</v>
-      </c>
       <c r="N15" t="n">
+        <v>0.00124989897313948</v>
+      </c>
+      <c r="O15" t="n">
         <v>0.360207488795103</v>
       </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
         <v>0.262157540379117</v>
       </c>
-      <c r="P15" t="n">
-        <v>21.9436428866523</v>
-      </c>
       <c r="Q15" t="n">
+        <v>0.150673562844058</v>
+      </c>
+      <c r="R15" t="n">
         <v>0.774978209490643</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>0.785998811501493</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>0.786357200370142</v>
       </c>
-      <c r="T15" t="n">
+      <c r="U15" t="n">
         <v>0.79447999684081</v>
       </c>
-      <c r="U15" t="n">
-        <v>0.472759228731968</v>
-      </c>
       <c r="V15" t="n">
-        <v>1.18632276222498</v>
+        <v>0.827091193491121</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.831990797465827</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" t="n">
+        <v>25810</v>
+      </c>
+      <c r="C16" t="n">
         <v>0.617869657620099</v>
       </c>
-      <c r="C16" t="n">
-        <v>0.00522190345325718</v>
-      </c>
       <c r="D16" t="n">
+        <v>0.017087872830346</v>
+      </c>
+      <c r="E16" t="n">
         <v>0.695393330472484</v>
       </c>
-      <c r="E16" t="n">
-        <v>0.00470096131762572</v>
-      </c>
       <c r="F16" t="n">
-        <v>0.47164635567494</v>
+        <v>0.0135996477610361</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00269226853909384</v>
+        <v>0.688982551274551</v>
       </c>
       <c r="H16" t="n">
+        <v>0.0256943023662428</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.609383735684052</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.685866938415752</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.675641435518982</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0.00257101062139269</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>0.00267788758712278</v>
       </c>
-      <c r="M16" t="n">
-        <v>0.222696039185922</v>
-      </c>
       <c r="N16" t="n">
+        <v>0.00169961795729649</v>
+      </c>
+      <c r="O16" t="n">
         <v>0.439441919813756</v>
       </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
         <v>0.37485559915329</v>
       </c>
-      <c r="P16" t="n">
-        <v>32.960684096419</v>
-      </c>
       <c r="Q16" t="n">
+        <v>0.251556205399238</v>
+      </c>
+      <c r="R16" t="n">
         <v>0.604135076013291</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
         <v>0.614632395354812</v>
       </c>
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>0.680827757597822</v>
       </c>
-      <c r="T16" t="n">
+      <c r="U16" t="n">
         <v>0.690906119233681</v>
       </c>
-      <c r="U16" t="n">
-        <v>0.239157198714575</v>
-      </c>
       <c r="V16" t="n">
-        <v>1.11212567232339</v>
+        <v>0.672310184322681</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.678972686715283</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" t="n">
+        <v>20705</v>
+      </c>
+      <c r="C17" t="n">
         <v>0.626815222002308</v>
       </c>
-      <c r="C17" t="n">
-        <v>0.00451612406309289</v>
-      </c>
       <c r="D17" t="n">
+        <v>0.0165383090547028</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.641698435858412</v>
       </c>
-      <c r="E17" t="n">
-        <v>0.00445899611611692</v>
-      </c>
       <c r="F17" t="n">
-        <v>0.402171423064658</v>
+        <v>0.0202010242142802</v>
       </c>
       <c r="G17" t="n">
-        <v>0.00218158049231036</v>
+        <v>0.580715172290505</v>
       </c>
       <c r="H17" t="n">
+        <v>0.0375914388310494</v>
+      </c>
+      <c r="I17" t="n">
         <v>0.613977858195642</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.648210177577909</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0.585302236064272</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0.00322688386575513</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>0.00333296035881704</v>
       </c>
-      <c r="M17" t="n">
-        <v>0.198484683707293</v>
-      </c>
       <c r="N17" t="n">
+        <v>0.00197934803042874</v>
+      </c>
+      <c r="O17" t="n">
         <v>0.542846995918053</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
         <v>0.497814440034349</v>
       </c>
-      <c r="P17" t="n">
-        <v>33.9114856355167</v>
-      </c>
       <c r="Q17" t="n">
+        <v>0.338175374783873</v>
+      </c>
+      <c r="R17" t="n">
         <v>0.60744525589236</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
         <v>0.620510460498923</v>
       </c>
-      <c r="S17" t="n">
+      <c r="T17" t="n">
         <v>0.641885485201029</v>
       </c>
-      <c r="T17" t="n">
+      <c r="U17" t="n">
         <v>0.654534869954789</v>
       </c>
-      <c r="U17" t="n">
-        <v>0.196272255997977</v>
-      </c>
       <c r="V17" t="n">
-        <v>0.974332216130567</v>
+        <v>0.581422713924631</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.589181758203912</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" t="n">
+        <v>21926</v>
+      </c>
+      <c r="C18" t="n">
         <v>0.685245060331529</v>
       </c>
-      <c r="C18" t="n">
-        <v>0.00572649188252539</v>
-      </c>
       <c r="D18" t="n">
+        <v>0.0123512039302643</v>
+      </c>
+      <c r="E18" t="n">
         <v>0.712605386539129</v>
       </c>
-      <c r="E18" t="n">
-        <v>0.00522795015880714</v>
-      </c>
       <c r="F18" t="n">
-        <v>0.519410573814983</v>
+        <v>0.0140467697706322</v>
       </c>
       <c r="G18" t="n">
-        <v>0.00234628875783029</v>
+        <v>0.79321122574917</v>
       </c>
       <c r="H18" t="n">
+        <v>0.0155451506052855</v>
+      </c>
+      <c r="I18" t="n">
         <v>0.711548390955164</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>0.707861024672471</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>0.823820104523769</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>0.00299701596993502</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>0.00259529550156573</v>
       </c>
-      <c r="M18" t="n">
-        <v>0.249156488427116</v>
-      </c>
       <c r="N18" t="n">
+        <v>0.00103290202517034</v>
+      </c>
+      <c r="O18" t="n">
         <v>0.364739142770301</v>
       </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
         <v>0.423390448898036</v>
       </c>
-      <c r="P18" t="n">
-        <v>30.2440407874178</v>
-      </c>
       <c r="Q18" t="n">
+        <v>0.125379560355284</v>
+      </c>
+      <c r="R18" t="n">
         <v>0.706461611772095</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>0.716635170138232</v>
       </c>
-      <c r="S18" t="n">
+      <c r="T18" t="n">
         <v>0.701986873371398</v>
       </c>
-      <c r="T18" t="n">
+      <c r="U18" t="n">
         <v>0.713735175973544</v>
       </c>
-      <c r="U18" t="n">
-        <v>0.335473387206621</v>
-      </c>
       <c r="V18" t="n">
-        <v>1.31216682184092</v>
+        <v>0.821795616554435</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.825844592493102</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" t="n">
+        <v>22157</v>
+      </c>
+      <c r="C19" t="n">
         <v>0.660324025291542</v>
       </c>
-      <c r="C19" t="n">
-        <v>0.00398655594671446</v>
-      </c>
       <c r="D19" t="n">
+        <v>0.017604216761652</v>
+      </c>
+      <c r="E19" t="n">
         <v>0.681126630761566</v>
       </c>
-      <c r="E19" t="n">
-        <v>0.00395011015429499</v>
-      </c>
       <c r="F19" t="n">
-        <v>0.443196443931544</v>
+        <v>0.0153696411160341</v>
       </c>
       <c r="G19" t="n">
-        <v>0.00199881982042142</v>
+        <v>0.654954459399649</v>
       </c>
       <c r="H19" t="n">
+        <v>0.0317156653658607</v>
+      </c>
+      <c r="I19" t="n">
         <v>0.650055774033806</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>0.680251933957271</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>0.659159066760244</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>0.002805812016169</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>0.00283870272538234</v>
       </c>
-      <c r="M19" t="n">
-        <v>0.200572948437639</v>
-      </c>
       <c r="N19" t="n">
+        <v>0.00186685755085523</v>
+      </c>
+      <c r="O19" t="n">
         <v>0.43668602584164</v>
       </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
         <v>0.412466598932924</v>
       </c>
-      <c r="P19" t="n">
-        <v>30.4286110215326</v>
-      </c>
       <c r="Q19" t="n">
+        <v>0.283218064500092</v>
+      </c>
+      <c r="R19" t="n">
         <v>0.644491916692056</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
         <v>0.655619631375555</v>
       </c>
-      <c r="S19" t="n">
+      <c r="T19" t="n">
         <v>0.674752542405579</v>
       </c>
-      <c r="T19" t="n">
+      <c r="U19" t="n">
         <v>0.685751325508962</v>
       </c>
-      <c r="U19" t="n">
-        <v>0.266036087822471</v>
-      </c>
       <c r="V19" t="n">
-        <v>1.05228204569802</v>
+        <v>0.655500025960568</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.66281810755992</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" t="n">
+        <v>22033</v>
+      </c>
+      <c r="C20" t="n">
         <v>0.603852094866208</v>
       </c>
-      <c r="C20" t="n">
-        <v>0.00709762068837437</v>
-      </c>
       <c r="D20" t="n">
+        <v>0.0189238272590431</v>
+      </c>
+      <c r="E20" t="n">
         <v>0.600319563285709</v>
       </c>
-      <c r="E20" t="n">
-        <v>0.00694734779284849</v>
-      </c>
       <c r="F20" t="n">
-        <v>0.358980109044214</v>
+        <v>0.0196868614274677</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00273990877517339</v>
+        <v>0.51538613346449</v>
       </c>
       <c r="H20" t="n">
+        <v>0.0447815377169688</v>
+      </c>
+      <c r="I20" t="n">
         <v>0.597313954514135</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>0.556423239324126</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>0.439344367434619</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>0.00331646182502219</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>0.00334363662860974</v>
       </c>
-      <c r="M20" t="n">
-        <v>0.107189625075493</v>
-      </c>
       <c r="N20" t="n">
+        <v>0.0023015751027254</v>
+      </c>
+      <c r="O20" t="n">
         <v>0.559778756772811</v>
       </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
         <v>0.596032227023914</v>
       </c>
-      <c r="P20" t="n">
-        <v>24.3976327047017</v>
-      </c>
       <c r="Q20" t="n">
+        <v>0.523865849507654</v>
+      </c>
+      <c r="R20" t="n">
         <v>0.59076042672206</v>
       </c>
-      <c r="R20" t="n">
+      <c r="S20" t="n">
         <v>0.60386748230621</v>
       </c>
-      <c r="S20" t="n">
+      <c r="T20" t="n">
         <v>0.549922974147082</v>
       </c>
-      <c r="T20" t="n">
+      <c r="U20" t="n">
         <v>0.562923504501169</v>
       </c>
-      <c r="U20" t="n">
-        <v>0.229252702286652</v>
-      </c>
       <c r="V20" t="n">
-        <v>0.649436032582586</v>
+        <v>0.434833280233277</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.443855454635961</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" t="n">
+        <v>22301</v>
+      </c>
+      <c r="C21" t="n">
         <v>0.633307603165205</v>
       </c>
-      <c r="C21" t="n">
-        <v>0.00469855510962364</v>
-      </c>
       <c r="D21" t="n">
+        <v>0.0120186893847372</v>
+      </c>
+      <c r="E21" t="n">
         <v>0.583664830603977</v>
       </c>
-      <c r="E21" t="n">
-        <v>0.00475472358264369</v>
-      </c>
       <c r="F21" t="n">
-        <v>0.362230089981039</v>
+        <v>0.0213788847566121</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00251457456332853</v>
+        <v>0.508845784809598</v>
       </c>
       <c r="H21" t="n">
+        <v>0.0410291353179988</v>
+      </c>
+      <c r="I21" t="n">
         <v>0.634096255422113</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>0.547911756027029</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>0.463658576529257</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>0.0030954398158163</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>0.00348133952728797</v>
       </c>
-      <c r="M21" t="n">
-        <v>0.0940485505915715</v>
-      </c>
       <c r="N21" t="n">
+        <v>0.00191529935778038</v>
+      </c>
+      <c r="O21" t="n">
         <v>0.549023826827437</v>
       </c>
-      <c r="O21" t="n">
+      <c r="P21" t="n">
         <v>0.564952254038441</v>
       </c>
-      <c r="P21" t="n">
-        <v>20.28400968997</v>
-      </c>
       <c r="Q21" t="n">
+        <v>0.413083992130042</v>
+      </c>
+      <c r="R21" t="n">
         <v>0.627272829948629</v>
       </c>
-      <c r="R21" t="n">
+      <c r="S21" t="n">
         <v>0.640919680895598</v>
       </c>
-      <c r="S21" t="n">
+      <c r="T21" t="n">
         <v>0.541844693988029</v>
       </c>
-      <c r="T21" t="n">
+      <c r="U21" t="n">
         <v>0.553978818066029</v>
       </c>
-      <c r="U21" t="n">
-        <v>0.279323417369777</v>
-      </c>
       <c r="V21" t="n">
-        <v>0.647993735688737</v>
+        <v>0.459904589788008</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0.467412563270507</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" t="n">
+        <v>23594</v>
+      </c>
+      <c r="C22" t="n">
         <v>0.616498477404802</v>
       </c>
-      <c r="C22" t="n">
-        <v>0.00447569468534665</v>
-      </c>
       <c r="D22" t="n">
+        <v>0.0124392626177386</v>
+      </c>
+      <c r="E22" t="n">
         <v>0.598489170126661</v>
       </c>
-      <c r="E22" t="n">
-        <v>0.00448823786983868</v>
-      </c>
       <c r="F22" t="n">
-        <v>0.375953761553124</v>
+        <v>0.018368440747994</v>
       </c>
       <c r="G22" t="n">
-        <v>0.00221330060747928</v>
+        <v>0.51067603598464</v>
       </c>
       <c r="H22" t="n">
+        <v>0.0346388612392504</v>
+      </c>
+      <c r="I22" t="n">
         <v>0.607996562858367</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>0.58768053430424</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>0.515055030560506</v>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>0.00326586006576449</v>
       </c>
-      <c r="L22" t="n">
+      <c r="M22" t="n">
         <v>0.00299047492118853</v>
       </c>
-      <c r="M22" t="n">
-        <v>0.162555350705141</v>
-      </c>
       <c r="N22" t="n">
+        <v>0.00155314374491218</v>
+      </c>
+      <c r="O22" t="n">
         <v>0.491857208391022</v>
       </c>
-      <c r="O22" t="n">
+      <c r="P22" t="n">
         <v>0.555720306378867</v>
       </c>
-      <c r="P22" t="n">
-        <v>31.5607733271222</v>
-      </c>
       <c r="Q22" t="n">
+        <v>0.301549087526042</v>
+      </c>
+      <c r="R22" t="n">
         <v>0.602135232012838</v>
       </c>
-      <c r="R22" t="n">
+      <c r="S22" t="n">
         <v>0.613857893703897</v>
       </c>
-      <c r="S22" t="n">
+      <c r="T22" t="n">
         <v>0.581279448575341</v>
       </c>
-      <c r="T22" t="n">
+      <c r="U22" t="n">
         <v>0.594081620033138</v>
       </c>
-      <c r="U22" t="n">
-        <v>0.196446543178429</v>
-      </c>
       <c r="V22" t="n">
-        <v>0.833663517942584</v>
+        <v>0.512010868820478</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0.518099192300534</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B23" t="n">
+        <v>24643</v>
+      </c>
+      <c r="C23" t="n">
         <v>0.712043123794436</v>
       </c>
-      <c r="C23" t="n">
-        <v>0.00516625017855865</v>
-      </c>
       <c r="D23" t="n">
+        <v>0.0134493484577902</v>
+      </c>
+      <c r="E23" t="n">
         <v>0.755758422101791</v>
       </c>
-      <c r="E23" t="n">
-        <v>0.00458243847153603</v>
-      </c>
       <c r="F23" t="n">
-        <v>0.51208157299055</v>
+        <v>0.0129542407060894</v>
       </c>
       <c r="G23" t="n">
-        <v>0.00257833317849086</v>
+        <v>0.750737463865294</v>
       </c>
       <c r="H23" t="n">
+        <v>0.0266990374084949</v>
+      </c>
+      <c r="I23" t="n">
         <v>0.717438195996371</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>0.745087399601091</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>0.749403991617224</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>0.00259054524987445</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>0.00289508774243836</v>
       </c>
-      <c r="M23" t="n">
-        <v>0.233568655736157</v>
-      </c>
       <c r="N23" t="n">
+        <v>0.00141749599024761</v>
+      </c>
+      <c r="O23" t="n">
         <v>0.403531308842247</v>
       </c>
-      <c r="O23" t="n">
+      <c r="P23" t="n">
         <v>0.347683406169718</v>
       </c>
-      <c r="P23" t="n">
-        <v>31.1672553587702</v>
-      </c>
       <c r="Q23" t="n">
+        <v>0.189149778504467</v>
+      </c>
+      <c r="R23" t="n">
         <v>0.711763824021192</v>
       </c>
-      <c r="R23" t="n">
+      <c r="S23" t="n">
         <v>0.72311256797155</v>
       </c>
-      <c r="S23" t="n">
+      <c r="T23" t="n">
         <v>0.740009930911337</v>
       </c>
-      <c r="T23" t="n">
+      <c r="U23" t="n">
         <v>0.750164868290845</v>
       </c>
-      <c r="U23" t="n">
-        <v>0.291609426374357</v>
-      </c>
       <c r="V23" t="n">
-        <v>1.20719855686009</v>
+        <v>0.746625699476339</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0.75218228375811</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B24" t="n">
+        <v>21036</v>
+      </c>
+      <c r="C24" t="n">
         <v>0.643996210204208</v>
       </c>
-      <c r="C24" t="n">
-        <v>0.00599942021699183</v>
-      </c>
       <c r="D24" t="n">
+        <v>0.0155144444056993</v>
+      </c>
+      <c r="E24" t="n">
         <v>0.64828565892758</v>
       </c>
-      <c r="E24" t="n">
-        <v>0.00574415650020371</v>
-      </c>
       <c r="F24" t="n">
-        <v>0.419566962918099</v>
+        <v>0.0163762216584876</v>
       </c>
       <c r="G24" t="n">
-        <v>0.00277405493154565</v>
+        <v>0.599558858836202</v>
       </c>
       <c r="H24" t="n">
+        <v>0.0271638626509951</v>
+      </c>
+      <c r="I24" t="n">
         <v>0.639330681291519</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>0.626722143122576</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>0.576169097415042</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>0.00303694450629423</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>0.00306790351104019</v>
       </c>
-      <c r="M24" t="n">
-        <v>0.145723933270154</v>
-      </c>
       <c r="N24" t="n">
+        <v>0.00181481385011351</v>
+      </c>
+      <c r="O24" t="n">
         <v>0.479861768066987</v>
       </c>
-      <c r="O24" t="n">
+      <c r="P24" t="n">
         <v>0.484575906503475</v>
       </c>
-      <c r="P24" t="n">
-        <v>25.2918689884512</v>
-      </c>
       <c r="Q24" t="n">
+        <v>0.314979379882677</v>
+      </c>
+      <c r="R24" t="n">
         <v>0.63331759040988</v>
       </c>
-      <c r="R24" t="n">
+      <c r="S24" t="n">
         <v>0.645343772173157</v>
       </c>
-      <c r="S24" t="n">
+      <c r="T24" t="n">
         <v>0.620769731890239</v>
       </c>
-      <c r="T24" t="n">
+      <c r="U24" t="n">
         <v>0.632674554354912</v>
       </c>
-      <c r="U24" t="n">
-        <v>0.29055018820554</v>
-      </c>
       <c r="V24" t="n">
-        <v>0.861788006624544</v>
+        <v>0.57261206226882</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0.579726132561265</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B25" t="n">
+        <v>28436</v>
+      </c>
+      <c r="C25" t="n">
         <v>0.545460811679429</v>
       </c>
-      <c r="C25" t="n">
-        <v>0.00353567021784675</v>
-      </c>
       <c r="D25" t="n">
+        <v>0.0127161449823412</v>
+      </c>
+      <c r="E25" t="n">
         <v>0.542326008201143</v>
       </c>
-      <c r="E25" t="n">
-        <v>0.00352347776574705</v>
-      </c>
       <c r="F25" t="n">
-        <v>0.310390379639101</v>
+        <v>0.0160972894521955</v>
       </c>
       <c r="G25" t="n">
-        <v>0.00156537072433953</v>
+        <v>0.404598674701664</v>
       </c>
       <c r="H25" t="n">
+        <v>0.0385571184925014</v>
+      </c>
+      <c r="I25" t="n">
         <v>0.545079597601623</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>0.518445365220124</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>0.385076627920173</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>0.0031033199016924</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>0.00266115520863512</v>
       </c>
-      <c r="M25" t="n">
-        <v>0.108861627629659</v>
-      </c>
       <c r="N25" t="n">
+        <v>0.00216478544037066</v>
+      </c>
+      <c r="O25" t="n">
         <v>0.488214055404814</v>
       </c>
-      <c r="O25" t="n">
+      <c r="P25" t="n">
         <v>0.598581858355465</v>
       </c>
-      <c r="P25" t="n">
-        <v>28.2701207335352</v>
-      </c>
       <c r="Q25" t="n">
+        <v>0.562170041859675</v>
+      </c>
+      <c r="R25" t="n">
         <v>0.539863733392698</v>
       </c>
-      <c r="R25" t="n">
+      <c r="S25" t="n">
         <v>0.550295461810547</v>
       </c>
-      <c r="S25" t="n">
+      <c r="T25" t="n">
         <v>0.512362858212807</v>
       </c>
-      <c r="T25" t="n">
+      <c r="U25" t="n">
         <v>0.524527872227441</v>
       </c>
-      <c r="U25" t="n">
-        <v>0.171707837766041</v>
-      </c>
       <c r="V25" t="n">
-        <v>0.598445418074305</v>
+        <v>0.380833648457047</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.3893196073833</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B26"/>
       <c r="C26"/>
@@ -2218,55 +2296,56 @@
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="H26" t="n">
+      <c r="H26"/>
+      <c r="I26" t="n">
         <v>0.716618950357581</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>0.741373240461102</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>0.863498245552782</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>0.0348687935198066</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>0.030933790595386</v>
       </c>
-      <c r="M26" t="n">
-        <v>0.266269000004038</v>
-      </c>
       <c r="N26" t="n">
+        <v>0.0124962577277612</v>
+      </c>
+      <c r="O26" t="n">
         <v>4.31663027888818</v>
       </c>
-      <c r="O26" t="n">
+      <c r="P26" t="n">
         <v>4.70327112132071</v>
       </c>
-      <c r="P26" t="n">
-        <v>30.8360788658675</v>
-      </c>
       <c r="Q26" t="n">
+        <v>1.44716654516901</v>
+      </c>
+      <c r="R26" t="n">
         <v>0.655988720790625</v>
       </c>
-      <c r="R26" t="n">
+      <c r="S26" t="n">
         <v>0.777249179924538</v>
       </c>
-      <c r="S26" t="n">
+      <c r="T26" t="n">
         <v>0.673030405162282</v>
       </c>
-      <c r="T26" t="n">
+      <c r="U26" t="n">
         <v>0.809716075759923</v>
       </c>
-      <c r="U26" t="n">
-        <v>0.341611005544867</v>
-      </c>
       <c r="V26" t="n">
-        <v>1.3853854855607</v>
+        <v>0.83900558040637</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.887990910699194</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B27"/>
       <c r="C27"/>
@@ -2274,55 +2353,56 @@
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27" t="n">
+      <c r="H27"/>
+      <c r="I27" t="n">
         <v>0.674813101041297</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>0.675041949588754</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>0.641524963502602</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>0.0395065860548887</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>0.0328945591194969</v>
       </c>
-      <c r="M27" t="n">
-        <v>0.273581980872965</v>
-      </c>
       <c r="N27" t="n">
+        <v>0.0219435378570595</v>
+      </c>
+      <c r="O27" t="n">
         <v>4.87461773767251</v>
       </c>
-      <c r="O27" t="n">
+      <c r="P27" t="n">
         <v>5.85246384746262</v>
       </c>
-      <c r="P27" t="n">
-        <v>42.6455705447939</v>
-      </c>
       <c r="Q27" t="n">
+        <v>3.42052750952231</v>
+      </c>
+      <c r="R27" t="n">
         <v>0.610339765167083</v>
       </c>
-      <c r="R27" t="n">
+      <c r="S27" t="n">
         <v>0.739286436915511</v>
       </c>
-      <c r="S27" t="n">
+      <c r="T27" t="n">
         <v>0.597609040921172</v>
       </c>
-      <c r="T27" t="n">
+      <c r="U27" t="n">
         <v>0.752474858256336</v>
       </c>
-      <c r="U27" t="n">
-        <v>0.10530428099159</v>
-      </c>
       <c r="V27" t="n">
-        <v>1.17774564601361</v>
+        <v>0.598515629302766</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.684534297702439</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -2330,55 +2410,56 @@
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
-      <c r="H28" t="n">
+      <c r="H28"/>
+      <c r="I28" t="n">
         <v>0.728783640612074</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>0.740311213456729</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>0.861163482610652</v>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>0.0346179289538455</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>0.0281971644818462</v>
       </c>
-      <c r="M28" t="n">
-        <v>0.227149154917128</v>
-      </c>
       <c r="N28" t="n">
+        <v>0.0132789208266223</v>
+      </c>
+      <c r="O28" t="n">
         <v>3.86907209637206</v>
       </c>
-      <c r="O28" t="n">
+      <c r="P28" t="n">
         <v>4.6761319191971</v>
       </c>
-      <c r="P28" t="n">
-        <v>26.3770073283317</v>
-      </c>
       <c r="Q28" t="n">
+        <v>1.54197444443031</v>
+      </c>
+      <c r="R28" t="n">
         <v>0.673517198227656</v>
       </c>
-      <c r="R28" t="n">
+      <c r="S28" t="n">
         <v>0.784050082996493</v>
       </c>
-      <c r="S28" t="n">
+      <c r="T28" t="n">
         <v>0.672460072707191</v>
       </c>
-      <c r="T28" t="n">
+      <c r="U28" t="n">
         <v>0.808162354206266</v>
       </c>
-      <c r="U28" t="n">
-        <v>0.415951138973082</v>
-      </c>
       <c r="V28" t="n">
-        <v>1.30637582624822</v>
+        <v>0.835136797790472</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.887190167430831</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
@@ -2386,55 +2467,56 @@
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29" t="n">
+      <c r="H29"/>
+      <c r="I29" t="n">
         <v>0.581046802900461</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>0.627805405405405</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>0.844209360580092</v>
       </c>
-      <c r="K29" t="n">
+      <c r="L29" t="n">
         <v>0.0580035365813083</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
         <v>0.0535874616100596</v>
       </c>
-      <c r="M29" t="n">
-        <v>0.12165853248952</v>
-      </c>
       <c r="N29" t="n">
+        <v>0.0304575015715116</v>
+      </c>
+      <c r="O29" t="n">
         <v>9.22257231991682</v>
       </c>
-      <c r="O29" t="n">
+      <c r="P29" t="n">
         <v>9.23909480260886</v>
       </c>
-      <c r="P29" t="n">
-        <v>14.4109433240497</v>
-      </c>
       <c r="Q29" t="n">
+        <v>3.60781377152498</v>
+      </c>
+      <c r="R29" t="n">
         <v>0.476015378144745</v>
       </c>
-      <c r="R29" t="n">
+      <c r="S29" t="n">
         <v>0.686078227656178</v>
       </c>
-      <c r="S29" t="n">
+      <c r="T29" t="n">
         <v>0.514118473706041</v>
       </c>
-      <c r="T29" t="n">
+      <c r="U29" t="n">
         <v>0.74149233710477</v>
       </c>
-      <c r="U29" t="n">
-        <v>0.605758636900634</v>
-      </c>
       <c r="V29" t="n">
-        <v>1.08266008425955</v>
+        <v>0.78451265749993</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0.903906063660255</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
@@ -2442,55 +2524,56 @@
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="H30" t="n">
+      <c r="H30"/>
+      <c r="I30" t="n">
         <v>0.75391440745423</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>0.77031886500913</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>0.953956548204336</v>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>0.0320161469350603</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>0.0334513327190158</v>
       </c>
-      <c r="M30" t="n">
-        <v>0.118353035793507</v>
-      </c>
       <c r="N30" t="n">
+        <v>0.00681614162371865</v>
+      </c>
+      <c r="O30" t="n">
         <v>4.43701995720868</v>
       </c>
-      <c r="O30" t="n">
+      <c r="P30" t="n">
         <v>4.1562200264537</v>
       </c>
-      <c r="P30" t="n">
-        <v>12.4065436750014</v>
-      </c>
       <c r="Q30" t="n">
+        <v>0.714512797941259</v>
+      </c>
+      <c r="R30" t="n">
         <v>0.68834979532496</v>
       </c>
-      <c r="R30" t="n">
+      <c r="S30" t="n">
         <v>0.819479019583501</v>
       </c>
-      <c r="S30" t="n">
+      <c r="T30" t="n">
         <v>0.707567217016412</v>
       </c>
-      <c r="T30" t="n">
+      <c r="U30" t="n">
         <v>0.833070513001849</v>
       </c>
-      <c r="U30" t="n">
-        <v>0.721984598049062</v>
-      </c>
       <c r="V30" t="n">
-        <v>1.18592849835961</v>
+        <v>0.940596910621847</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0.967316185786824</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -2498,55 +2581,56 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" t="n">
+      <c r="H31"/>
+      <c r="I31" t="n">
         <v>0.778394955788531</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>0.804945715031899</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>0.961908741558781</v>
       </c>
-      <c r="K31" t="n">
+      <c r="L31" t="n">
         <v>0.0270950772561376</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
         <v>0.025156712332445</v>
       </c>
-      <c r="M31" t="n">
-        <v>0.137988604712299</v>
-      </c>
       <c r="N31" t="n">
+        <v>0.00573705980106885</v>
+      </c>
+      <c r="O31" t="n">
         <v>3.23186990683421</v>
       </c>
-      <c r="O31" t="n">
+      <c r="P31" t="n">
         <v>3.36607509676151</v>
       </c>
-      <c r="P31" t="n">
-        <v>14.3452906445873</v>
-      </c>
       <c r="Q31" t="n">
+        <v>0.596424541456178</v>
+      </c>
+      <c r="R31" t="n">
         <v>0.729087799616939</v>
       </c>
-      <c r="R31" t="n">
+      <c r="S31" t="n">
         <v>0.827702111960123</v>
       </c>
-      <c r="S31" t="n">
+      <c r="T31" t="n">
         <v>0.75183936360987</v>
       </c>
-      <c r="T31" t="n">
+      <c r="U31" t="n">
         <v>0.858052066453929</v>
       </c>
-      <c r="U31" t="n">
-        <v>0.691451076322674</v>
-      </c>
       <c r="V31" t="n">
-        <v>1.23236640679489</v>
+        <v>0.950664104348686</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.973153378768876</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -2554,55 +2638,56 @@
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32" t="n">
+      <c r="H32"/>
+      <c r="I32" t="n">
         <v>0.727860705106073</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>0.709114589327502</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>0.850898837610772</v>
       </c>
-      <c r="K32" t="n">
+      <c r="L32" t="n">
         <v>0.0367773481078161</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
         <v>0.0303442538926168</v>
       </c>
-      <c r="M32" t="n">
-        <v>0.185996675990196</v>
-      </c>
       <c r="N32" t="n">
+        <v>0.0121863206782744</v>
+      </c>
+      <c r="O32" t="n">
         <v>4.16896442956</v>
       </c>
-      <c r="O32" t="n">
+      <c r="P32" t="n">
         <v>5.18637589203944</v>
       </c>
-      <c r="P32" t="n">
-        <v>21.858847111891</v>
-      </c>
       <c r="Q32" t="n">
+        <v>1.43217032855424</v>
+      </c>
+      <c r="R32" t="n">
         <v>0.668385967476544</v>
       </c>
-      <c r="R32" t="n">
+      <c r="S32" t="n">
         <v>0.787335442735602</v>
       </c>
-      <c r="S32" t="n">
+      <c r="T32" t="n">
         <v>0.637030987036183</v>
       </c>
-      <c r="T32" t="n">
+      <c r="U32" t="n">
         <v>0.781198191618822</v>
       </c>
-      <c r="U32" t="n">
-        <v>0.486345352669988</v>
-      </c>
       <c r="V32" t="n">
-        <v>1.21545232255156</v>
+        <v>0.827013649081354</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.87478402614019</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -2610,55 +2695,56 @@
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33"/>
-      <c r="H33" t="n">
+      <c r="H33"/>
+      <c r="I33" t="n">
         <v>0.806954413652137</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>0.82915862527927</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>0.979626847934591</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L33" t="n">
         <v>0.0240508973905873</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>0.0260115006088414</v>
       </c>
-      <c r="M33" t="n">
-        <v>0.109601031603587</v>
-      </c>
       <c r="N33" t="n">
+        <v>0.00323359911343952</v>
+      </c>
+      <c r="O33" t="n">
         <v>3.22341636265645</v>
       </c>
-      <c r="O33" t="n">
+      <c r="P33" t="n">
         <v>2.90063887142062</v>
       </c>
-      <c r="P33" t="n">
-        <v>11.1880387756487</v>
-      </c>
       <c r="Q33" t="n">
+        <v>0.33008477873561</v>
+      </c>
+      <c r="R33" t="n">
         <v>0.755971872458808</v>
       </c>
-      <c r="R33" t="n">
+      <c r="S33" t="n">
         <v>0.857936954845466</v>
       </c>
-      <c r="S33" t="n">
+      <c r="T33" t="n">
         <v>0.782018866393719</v>
       </c>
-      <c r="T33" t="n">
+      <c r="U33" t="n">
         <v>0.876298384164821</v>
       </c>
-      <c r="U33" t="n">
-        <v>0.764808825991561</v>
-      </c>
       <c r="V33" t="n">
-        <v>1.19444486987762</v>
+        <v>0.97328899367225</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.985964702196933</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -2666,50 +2752,51 @@
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34"/>
-      <c r="H34" t="n">
+      <c r="H34"/>
+      <c r="I34" t="n">
         <v>0.79637964195887</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>0.84860080738909</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>0.957876693509183</v>
       </c>
-      <c r="K34" t="n">
+      <c r="L34" t="n">
         <v>0.0259547617964963</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
         <v>0.022669706968705</v>
       </c>
-      <c r="M34" t="n">
-        <v>0.184657162511518</v>
-      </c>
       <c r="N34" t="n">
+        <v>0.00544756565094376</v>
+      </c>
+      <c r="O34" t="n">
         <v>2.84659548967675</v>
       </c>
-      <c r="O34" t="n">
+      <c r="P34" t="n">
         <v>3.05853607143645</v>
       </c>
-      <c r="P34" t="n">
-        <v>19.2777592108464</v>
-      </c>
       <c r="Q34" t="n">
+        <v>0.568712621139845</v>
+      </c>
+      <c r="R34" t="n">
         <v>0.751947016300208</v>
       </c>
-      <c r="R34" t="n">
+      <c r="S34" t="n">
         <v>0.840812267617531</v>
       </c>
-      <c r="S34" t="n">
+      <c r="T34" t="n">
         <v>0.797729474267957</v>
       </c>
-      <c r="T34" t="n">
+      <c r="U34" t="n">
         <v>0.899472140510222</v>
       </c>
-      <c r="U34" t="n">
-        <v>0.595948654986609</v>
-      </c>
       <c r="V34" t="n">
-        <v>1.31980473203176</v>
+        <v>0.947199464833334</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.968553922185033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de tablas de salida dir_cv*100 -SG
</commit_message>
<xml_diff>
--- a/Frecuentista_depto/COL/Output/Comparando_dir_censo_sae/Estimacion_depto.xlsx
+++ b/Frecuentista_depto/COL/Output/Comparando_dir_censo_sae/Estimacion_depto.xlsx
@@ -593,19 +593,19 @@
         <v>0.646031468946502</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0122363159273592</v>
+        <v>1.22363159273592</v>
       </c>
       <c r="E2" t="n">
         <v>0.492689294407173</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0234368227720502</v>
+        <v>2.34368227720502</v>
       </c>
       <c r="G2" t="n">
         <v>0.455453832969968</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0432303687012702</v>
+        <v>4.32303687012702</v>
       </c>
       <c r="I2" t="n">
         <v>0.649198730991558</v>
@@ -664,19 +664,19 @@
         <v>0.531246079338757</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0102559205399277</v>
+        <v>1.02559205399277</v>
       </c>
       <c r="E3" t="n">
         <v>0.616411361201528</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0102454935547865</v>
+        <v>1.02454935547865</v>
       </c>
       <c r="G3" t="n">
         <v>0.453295906236899</v>
       </c>
       <c r="H3" t="n">
-        <v>0.016948506765515</v>
+        <v>1.6948506765515</v>
       </c>
       <c r="I3" t="n">
         <v>0.542272216357288</v>
@@ -735,19 +735,19 @@
         <v>0.573541855393646</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00639841023975061</v>
+        <v>0.639841023975061</v>
       </c>
       <c r="E4" t="n">
         <v>0.427985524029992</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00870340887289321</v>
+        <v>0.870340887289321</v>
       </c>
       <c r="G4" t="n">
         <v>0.284482254225353</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0161562512835023</v>
+        <v>1.61562512835023</v>
       </c>
       <c r="I4" t="n">
         <v>0.58431274528565</v>
@@ -806,19 +806,19 @@
         <v>0.652883565191465</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0133588636411288</v>
+        <v>1.33588636411288</v>
       </c>
       <c r="E5" t="n">
         <v>0.671537453556966</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0155427096797639</v>
+        <v>1.55427096797639</v>
       </c>
       <c r="G5" t="n">
         <v>0.631695350572367</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0220955045120061</v>
+        <v>2.20955045120061</v>
       </c>
       <c r="I5" t="n">
         <v>0.647318447403382</v>
@@ -877,19 +877,19 @@
         <v>0.667923343012017</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0137434547594035</v>
+        <v>1.37434547594035</v>
       </c>
       <c r="E6" t="n">
         <v>0.610926546733503</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0247331419747194</v>
+        <v>2.47331419747194</v>
       </c>
       <c r="G6" t="n">
         <v>0.615385585877384</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0409827146443487</v>
+        <v>4.09827146443487</v>
       </c>
       <c r="I6" t="n">
         <v>0.699363159911048</v>
@@ -948,19 +948,19 @@
         <v>0.643218101194196</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0161790037431009</v>
+        <v>1.61790037431009</v>
       </c>
       <c r="E7" t="n">
         <v>0.535410487497843</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0339916807302881</v>
+        <v>3.39916807302881</v>
       </c>
       <c r="G7" t="n">
         <v>0.521485471371696</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0533490420681228</v>
+        <v>5.33490420681228</v>
       </c>
       <c r="I7" t="n">
         <v>0.623141254306129</v>
@@ -1019,19 +1019,19 @@
         <v>0.72213008434979</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0163753716614274</v>
+        <v>1.63753716614274</v>
       </c>
       <c r="E8" t="n">
         <v>0.763437135211824</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0144538919809412</v>
+        <v>1.44538919809412</v>
       </c>
       <c r="G8" t="n">
         <v>0.796493205161876</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0163780251745944</v>
+        <v>1.63780251745944</v>
       </c>
       <c r="I8" t="n">
         <v>0.746260244142302</v>
@@ -1090,19 +1090,19 @@
         <v>0.667383179365901</v>
       </c>
       <c r="D9" t="n">
-        <v>0.020919322646248</v>
+        <v>2.0919322646248</v>
       </c>
       <c r="E9" t="n">
         <v>0.706238725903718</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0200125432188873</v>
+        <v>2.00125432188873</v>
       </c>
       <c r="G9" t="n">
         <v>0.736748961415124</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0237836869092163</v>
+        <v>2.37836869092163</v>
       </c>
       <c r="I9" t="n">
         <v>0.739854415825333</v>
@@ -1161,19 +1161,19 @@
         <v>0.669223003220315</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0151098190021899</v>
+        <v>1.51098190021899</v>
       </c>
       <c r="E10" t="n">
         <v>0.706879692595728</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0124185107950698</v>
+        <v>1.24185107950698</v>
       </c>
       <c r="G10" t="n">
         <v>0.662764350369233</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0227072693332446</v>
+        <v>2.27072693332446</v>
       </c>
       <c r="I10" t="n">
         <v>0.649918885562665</v>
@@ -1232,19 +1232,19 @@
         <v>0.633572227796042</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0148768169633349</v>
+        <v>1.48768169633349</v>
       </c>
       <c r="E11" t="n">
         <v>0.733469683582859</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0119871335787648</v>
+        <v>1.19871335787648</v>
       </c>
       <c r="G11" t="n">
         <v>0.714470429787794</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0234502470624658</v>
+        <v>2.34502470624658</v>
       </c>
       <c r="I11" t="n">
         <v>0.643772520705782</v>
@@ -1303,19 +1303,19 @@
         <v>0.615507923256318</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0131978838012724</v>
+        <v>1.31978838012724</v>
       </c>
       <c r="E12" t="n">
         <v>0.56398402183457</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0296568739387281</v>
+        <v>2.96568739387281</v>
       </c>
       <c r="G12" t="n">
         <v>0.552134997456974</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0374849182064167</v>
+        <v>3.74849182064167</v>
       </c>
       <c r="I12" t="n">
         <v>0.62065986148731</v>
@@ -1374,19 +1374,19 @@
         <v>0.716158353532741</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0199853842235368</v>
+        <v>1.99853842235368</v>
       </c>
       <c r="E13" t="n">
         <v>0.753839305688845</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0191776743361688</v>
+        <v>1.91776743361688</v>
       </c>
       <c r="G13" t="n">
         <v>0.927914308185246</v>
       </c>
       <c r="H13" t="n">
-        <v>0.014034897498135</v>
+        <v>1.4034897498135</v>
       </c>
       <c r="I13" t="n">
         <v>0.766862976337199</v>
@@ -1445,19 +1445,19 @@
         <v>0.674345694284293</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0112708711710327</v>
+        <v>1.12708711710327</v>
       </c>
       <c r="E14" t="n">
         <v>0.678515266920817</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0181938890757664</v>
+        <v>1.81938890757664</v>
       </c>
       <c r="G14" t="n">
         <v>0.613260439316588</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0302998226552923</v>
+        <v>3.02998226552923</v>
       </c>
       <c r="I14" t="n">
         <v>0.682143343498224</v>
@@ -1516,19 +1516,19 @@
         <v>0.720280981493297</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0190851050289625</v>
+        <v>1.90851050289625</v>
       </c>
       <c r="E15" t="n">
         <v>0.761909547287528</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0208995086789547</v>
+        <v>2.08995086789547</v>
       </c>
       <c r="G15" t="n">
         <v>0.823982459272416</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0185139071518655</v>
+        <v>1.85139071518655</v>
       </c>
       <c r="I15" t="n">
         <v>0.780488510496068</v>
@@ -1587,19 +1587,19 @@
         <v>0.617869657620099</v>
       </c>
       <c r="D16" t="n">
-        <v>0.017087872830346</v>
+        <v>1.7087872830346</v>
       </c>
       <c r="E16" t="n">
         <v>0.695393330472484</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0135996477610361</v>
+        <v>1.35996477610361</v>
       </c>
       <c r="G16" t="n">
         <v>0.688982551274551</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0256943023662428</v>
+        <v>2.56943023662428</v>
       </c>
       <c r="I16" t="n">
         <v>0.609383735684052</v>
@@ -1658,19 +1658,19 @@
         <v>0.626815222002308</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0165383090547028</v>
+        <v>1.65383090547028</v>
       </c>
       <c r="E17" t="n">
         <v>0.641698435858412</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0202010242142802</v>
+        <v>2.02010242142802</v>
       </c>
       <c r="G17" t="n">
         <v>0.580715172290505</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0375914388310494</v>
+        <v>3.75914388310494</v>
       </c>
       <c r="I17" t="n">
         <v>0.613977858195642</v>
@@ -1729,19 +1729,19 @@
         <v>0.685245060331529</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0123512039302643</v>
+        <v>1.23512039302643</v>
       </c>
       <c r="E18" t="n">
         <v>0.712605386539129</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0140467697706322</v>
+        <v>1.40467697706322</v>
       </c>
       <c r="G18" t="n">
         <v>0.79321122574917</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0155451506052855</v>
+        <v>1.55451506052855</v>
       </c>
       <c r="I18" t="n">
         <v>0.711548390955164</v>
@@ -1800,19 +1800,19 @@
         <v>0.660324025291542</v>
       </c>
       <c r="D19" t="n">
-        <v>0.017604216761652</v>
+        <v>1.7604216761652</v>
       </c>
       <c r="E19" t="n">
         <v>0.681126630761566</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0153696411160341</v>
+        <v>1.53696411160341</v>
       </c>
       <c r="G19" t="n">
         <v>0.654954459399649</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0317156653658607</v>
+        <v>3.17156653658607</v>
       </c>
       <c r="I19" t="n">
         <v>0.650055774033806</v>
@@ -1871,19 +1871,19 @@
         <v>0.603852094866208</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0189238272590431</v>
+        <v>1.89238272590431</v>
       </c>
       <c r="E20" t="n">
         <v>0.600319563285709</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0196868614274677</v>
+        <v>1.96868614274677</v>
       </c>
       <c r="G20" t="n">
         <v>0.51538613346449</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0447815377169688</v>
+        <v>4.47815377169688</v>
       </c>
       <c r="I20" t="n">
         <v>0.597313954514135</v>
@@ -1942,19 +1942,19 @@
         <v>0.633307603165205</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0120186893847372</v>
+        <v>1.20186893847372</v>
       </c>
       <c r="E21" t="n">
         <v>0.583664830603977</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0213788847566121</v>
+        <v>2.13788847566121</v>
       </c>
       <c r="G21" t="n">
         <v>0.508845784809598</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0410291353179988</v>
+        <v>4.10291353179988</v>
       </c>
       <c r="I21" t="n">
         <v>0.634096255422113</v>
@@ -2013,19 +2013,19 @@
         <v>0.616498477404802</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0124392626177386</v>
+        <v>1.24392626177386</v>
       </c>
       <c r="E22" t="n">
         <v>0.598489170126661</v>
       </c>
       <c r="F22" t="n">
-        <v>0.018368440747994</v>
+        <v>1.8368440747994</v>
       </c>
       <c r="G22" t="n">
         <v>0.51067603598464</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0346388612392504</v>
+        <v>3.46388612392504</v>
       </c>
       <c r="I22" t="n">
         <v>0.607996562858367</v>
@@ -2084,19 +2084,19 @@
         <v>0.712043123794436</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0134493484577902</v>
+        <v>1.34493484577902</v>
       </c>
       <c r="E23" t="n">
         <v>0.755758422101791</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0129542407060894</v>
+        <v>1.29542407060894</v>
       </c>
       <c r="G23" t="n">
         <v>0.750737463865294</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0266990374084949</v>
+        <v>2.66990374084949</v>
       </c>
       <c r="I23" t="n">
         <v>0.717438195996371</v>
@@ -2155,19 +2155,19 @@
         <v>0.643996210204208</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0155144444056993</v>
+        <v>1.55144444056993</v>
       </c>
       <c r="E24" t="n">
         <v>0.64828565892758</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0163762216584876</v>
+        <v>1.63762216584876</v>
       </c>
       <c r="G24" t="n">
         <v>0.599558858836202</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0271638626509951</v>
+        <v>2.71638626509951</v>
       </c>
       <c r="I24" t="n">
         <v>0.639330681291519</v>
@@ -2226,19 +2226,19 @@
         <v>0.545460811679429</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0127161449823412</v>
+        <v>1.27161449823412</v>
       </c>
       <c r="E25" t="n">
         <v>0.542326008201143</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0160972894521955</v>
+        <v>1.60972894521955</v>
       </c>
       <c r="G25" t="n">
         <v>0.404598674701664</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0385571184925014</v>
+        <v>3.85571184925014</v>
       </c>
       <c r="I25" t="n">
         <v>0.545079597601623</v>

</xml_diff>